<commit_message>
Updated with the latest moderation budgets
</commit_message>
<xml_diff>
--- a/Main/Source/Databases/The Guide/DBScripts/KPI Reports/kpi March-May 2012.xlsx
+++ b/Main/Source/Databases/The Guide/DBScripts/KPI Reports/kpi March-May 2012.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="10080" windowHeight="9936" activeTab="1"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="10080" windowHeight="9936"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="2" r:id="rId1"/>
@@ -807,11 +807,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104308736"/>
-        <c:axId val="104310272"/>
+        <c:axId val="51691520"/>
+        <c:axId val="51693056"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="104308736"/>
+        <c:axId val="51691520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,14 +821,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104310272"/>
+        <c:crossAx val="51693056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="104310272"/>
+        <c:axId val="51693056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104308736"/>
+        <c:crossAx val="51691520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -970,8 +970,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104337792"/>
-        <c:axId val="104336000"/>
+        <c:axId val="51868032"/>
+        <c:axId val="51858048"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1053,11 +1053,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104332672"/>
-        <c:axId val="104334464"/>
+        <c:axId val="51854720"/>
+        <c:axId val="51856512"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="104332672"/>
+        <c:axId val="51854720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,14 +1067,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104334464"/>
+        <c:crossAx val="51856512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="104334464"/>
+        <c:axId val="51856512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1085,12 +1085,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104332672"/>
+        <c:crossAx val="51854720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104336000"/>
+        <c:axId val="51858048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1100,12 +1100,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104337792"/>
+        <c:crossAx val="51868032"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="104337792"/>
+        <c:axId val="51868032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,7 +1115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104336000"/>
+        <c:crossAx val="51858048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1227,8 +1227,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104588800"/>
-        <c:axId val="104590336"/>
+        <c:axId val="52454912"/>
+        <c:axId val="52456448"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1301,11 +1301,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104588800"/>
-        <c:axId val="104590336"/>
+        <c:axId val="52454912"/>
+        <c:axId val="52456448"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="104588800"/>
+        <c:axId val="52454912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,14 +1315,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104590336"/>
+        <c:crossAx val="52456448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="104590336"/>
+        <c:axId val="52456448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,14 +1333,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104588800"/>
+        <c:crossAx val="52454912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1744,10 +1743,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4416" topLeftCell="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4416" topLeftCell="K1" activePane="topRight"/>
       <selection activeCell="O11" sqref="O11"/>
-      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="topRight" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2073,27 +2072,27 @@
         <v>1</v>
       </c>
       <c r="J6" s="26">
-        <f>I6</f>
+        <f t="shared" ref="J6:O6" si="0">I6</f>
         <v>1</v>
       </c>
       <c r="K6" s="26">
-        <f>J6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L6" s="26">
-        <f>K6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M6" s="26">
-        <f>L6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N6" s="26">
-        <f>M6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O6" s="26">
-        <f>N6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P6" s="26"/>
@@ -2367,15 +2366,15 @@
       </c>
       <c r="M10" s="31">
         <f>Data!G96/Data!G95</f>
-        <v>0.23318920038260149</v>
+        <v>0.28448590389602707</v>
       </c>
       <c r="N10" s="31">
         <f>Data!G103/Data!G102</f>
-        <v>0.21390213016145809</v>
+        <v>0.3094777260187237</v>
       </c>
       <c r="O10" s="31">
         <f>Data!G110/Data!G109</f>
-        <v>0.26005619460267887</v>
+        <v>0.41425638375085222</v>
       </c>
       <c r="P10" s="31"/>
       <c r="Q10" s="31"/>
@@ -2466,12 +2465,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3924" ySplit="2304" topLeftCell="F92" activePane="bottomRight"/>
       <selection activeCell="K4" sqref="K4"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomRight" activeCell="G108" sqref="G108"/>
+      <selection pane="bottomRight" activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3781,7 +3780,7 @@
         <v>16</v>
       </c>
       <c r="G96" s="48">
-        <v>23647.95</v>
+        <v>28850</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -3871,7 +3870,7 @@
         <v>16</v>
       </c>
       <c r="G103" s="48">
-        <v>23647.95</v>
+        <v>34214.31</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -3961,7 +3960,7 @@
         <v>16</v>
       </c>
       <c r="G110" s="48">
-        <v>23647.95</v>
+        <v>37669.99</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>